<commit_message>
code status as of green light moment
minor modifications
</commit_message>
<xml_diff>
--- a/analysis/q_a_level.xlsx
+++ b/analysis/q_a_level.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P.A. Ruben\Desktop\thesis SEC\1 - SE data\gis.SE.thesis\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131D9222-AF0E-41B1-AF2A-FE253497E15B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3E46E2-A796-498C-9285-BF09C3C522EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="1" xr2:uid="{1AA999AD-7864-4AC7-96FB-0556B191E784}"/>
+    <workbookView xWindow="24" yWindow="624" windowWidth="23016" windowHeight="12336" activeTab="1" xr2:uid="{1AA999AD-7864-4AC7-96FB-0556B191E784}"/>
   </bookViews>
   <sheets>
     <sheet name="old_2" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">old!$A$1:$G$53</definedName>
     <definedName name="ExternalData_2" localSheetId="0" hidden="1">old_2!$A$1:$G$53</definedName>
-    <definedName name="ExternalData_2" localSheetId="1" hidden="1">Sheet5!$A$1:$G$49</definedName>
+    <definedName name="ExternalData_2" localSheetId="1" hidden="1">Sheet5!$A$1:$G$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="31">
   <si>
     <t>high_interaction</t>
   </si>
@@ -137,11 +137,44 @@
   <si>
     <t>with code &amp; image &amp; ref</t>
   </si>
+  <si>
+    <t>all questions</t>
+  </si>
+  <si>
+    <t>with image</t>
+  </si>
+  <si>
+    <t>low interaction [%]</t>
+  </si>
+  <si>
+    <t>total number</t>
+  </si>
+  <si>
+    <t>1 high interaction chains [%]</t>
+  </si>
+  <si>
+    <t>2 high interaction chains [%]</t>
+  </si>
+  <si>
+    <t>with ext ref</t>
+  </si>
+  <si>
+    <t>all three</t>
+  </si>
+  <si>
+    <t>all answers</t>
+  </si>
+  <si>
+    <t>with code snippet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,10 +212,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -307,12 +341,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2553C6D7-3975-4665-90D5-8B3938DCB568}" name="q_a_content_analysis_corr" displayName="q_a_content_analysis_corr" ref="A1:G53" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G53" xr:uid="{9A206BB7-C7A8-40FF-9EE9-B0B763CE84B0}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{794C7DA1-23A8-4650-95BC-CE0F64AA404C}" uniqueName="1" name="answer" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{A9030AA6-80E5-4DF1-9AE5-D84A8BFD2C23}" uniqueName="2" name="high_interaction" queryTableFieldId="2" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{628E6078-D308-455C-9153-CE1B2EEE21FD}" uniqueName="3" name="very_high_interaction" queryTableFieldId="3" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{39DBD213-9307-4F86-9E99-0882E70510AF}" uniqueName="4" name="code_present" queryTableFieldId="4" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{05CBCD3D-8795-436B-911B-0C8476A02F19}" uniqueName="5" name="ext_ref_present" queryTableFieldId="5" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{D49E0ED9-9B8D-4D14-909B-5376645DD037}" uniqueName="6" name="img_present" queryTableFieldId="6" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{794C7DA1-23A8-4650-95BC-CE0F64AA404C}" uniqueName="1" name="answer" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{A9030AA6-80E5-4DF1-9AE5-D84A8BFD2C23}" uniqueName="2" name="high_interaction" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{628E6078-D308-455C-9153-CE1B2EEE21FD}" uniqueName="3" name="very_high_interaction" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{39DBD213-9307-4F86-9E99-0882E70510AF}" uniqueName="4" name="code_present" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{05CBCD3D-8795-436B-911B-0C8476A02F19}" uniqueName="5" name="ext_ref_present" queryTableFieldId="5" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{D49E0ED9-9B8D-4D14-909B-5376645DD037}" uniqueName="6" name="img_present" queryTableFieldId="6" dataDxfId="12"/>
     <tableColumn id="7" xr3:uid="{FB66BD83-7219-44AF-821F-A950296B9E93}" uniqueName="7" name="count" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -320,15 +354,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D6A0B0EB-5EE6-46C1-AE28-08A683CEDF5C}" name="q_a_content_analysis_corr__4" displayName="q_a_content_analysis_corr__4" ref="A1:G49" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G49" xr:uid="{6B9DB631-674C-4E88-B107-D9EB3B270109}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D6A0B0EB-5EE6-46C1-AE28-08A683CEDF5C}" name="q_a_content_analysis_corr__4" displayName="q_a_content_analysis_corr__4" ref="A1:G50" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G50" xr:uid="{6B9DB631-674C-4E88-B107-D9EB3B270109}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{453A782E-0A24-450B-84CF-AC2AAA0AC8B9}" uniqueName="1" name="answer" queryTableFieldId="1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C9A5FFAA-62A4-4560-A4F9-D87DCBCE1E7E}" uniqueName="2" name="high_interaction" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{FA1EAC45-7E33-4EC1-8FB8-EA5D9791EF46}" uniqueName="3" name="very_high_interaction" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{C02B3316-F8CB-48AB-BA11-51E3CD59BA26}" uniqueName="4" name="code_present" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E14E8B61-E437-4166-A98C-183FCCDB73E5}" uniqueName="5" name="ext_ref_present" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{934A31D5-C7B9-48E2-8F74-B02F9E0EDFA7}" uniqueName="6" name="img_present" queryTableFieldId="6" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{453A782E-0A24-450B-84CF-AC2AAA0AC8B9}" uniqueName="1" name="answer" queryTableFieldId="1" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C9A5FFAA-62A4-4560-A4F9-D87DCBCE1E7E}" uniqueName="2" name="high_interaction" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{FA1EAC45-7E33-4EC1-8FB8-EA5D9791EF46}" uniqueName="3" name="very_high_interaction" queryTableFieldId="3" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{C02B3316-F8CB-48AB-BA11-51E3CD59BA26}" uniqueName="4" name="code_present" queryTableFieldId="4" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E14E8B61-E437-4166-A98C-183FCCDB73E5}" uniqueName="5" name="ext_ref_present" queryTableFieldId="5" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{934A31D5-C7B9-48E2-8F74-B02F9E0EDFA7}" uniqueName="6" name="img_present" queryTableFieldId="6" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{319F78A3-DF20-46F5-B28A-8734753F2EC7}" uniqueName="7" name="count" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -339,12 +373,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F20C134-6AF1-4C7C-897B-6F98C89E59D2}" name="q_a_content_analysis__3" displayName="q_a_content_analysis__3" ref="A1:G53" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G53" xr:uid="{FB1B496D-B752-45AF-A9D5-EE1C99AB5439}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CD2D70CC-1A62-4838-B0DE-5BC683BD58A3}" uniqueName="1" name="answer" queryTableFieldId="1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{28154A6A-17CB-439E-822A-FCE8CC9212B6}" uniqueName="2" name="high_interaction" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{A2E39340-21AD-4588-9FD6-7B13DA935526}" uniqueName="3" name="very_high_interaction" queryTableFieldId="3" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F47F3A19-C7AA-4918-A237-3CB520EEFED0}" uniqueName="4" name="code_present" queryTableFieldId="4" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{F5FC88A0-9896-4022-B549-BB156F6608D9}" uniqueName="5" name="ext_ref_present" queryTableFieldId="5" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{12C88F32-DE17-46E2-990E-1742A99EE582}" uniqueName="6" name="img_present" queryTableFieldId="6" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{CD2D70CC-1A62-4838-B0DE-5BC683BD58A3}" uniqueName="1" name="answer" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{28154A6A-17CB-439E-822A-FCE8CC9212B6}" uniqueName="2" name="high_interaction" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{A2E39340-21AD-4588-9FD6-7B13DA935526}" uniqueName="3" name="very_high_interaction" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F47F3A19-C7AA-4918-A237-3CB520EEFED0}" uniqueName="4" name="code_present" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{F5FC88A0-9896-4022-B549-BB156F6608D9}" uniqueName="5" name="ext_ref_present" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{12C88F32-DE17-46E2-990E-1742A99EE582}" uniqueName="6" name="img_present" queryTableFieldId="6" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{A1805335-00FD-4860-B872-456882BE12D2}" uniqueName="7" name="count" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2263,10 +2297,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C53744-9D9A-44EF-AF74-C5C1EB79D41C}">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2278,6 +2312,8 @@
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2342,6 +2378,10 @@
         <f>J2/($J$2+$J$4)</f>
         <v>5.8801023957260917E-2</v>
       </c>
+      <c r="L2">
+        <f>J2+J4</f>
+        <v>143756</v>
+      </c>
       <c r="M2">
         <f>SUMIFS($G:$G, $A:$A, "=f", $B:$B, "=t")</f>
         <v>5556</v>
@@ -2350,6 +2390,10 @@
         <f>M2/(M2+M4)</f>
         <v>9.0139199844251922E-2</v>
       </c>
+      <c r="O2">
+        <f>M2+M4</f>
+        <v>61638</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2384,13 +2428,21 @@
         <f t="shared" ref="K3:K4" si="0">J3/($J$2+$J$4)</f>
         <v>2.8033612510086534E-3</v>
       </c>
+      <c r="L3">
+        <f>J2-J3</f>
+        <v>8050</v>
+      </c>
       <c r="M3">
         <f>SUMIFS($G:$G, $A:$A, "=f", $C:$C, "=t")</f>
         <v>625</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N4" si="1">M3/SUM($M$2:$M$4)</f>
+        <f t="shared" ref="N3" si="1">M3/SUM($M$2:$M$4)</f>
         <v>1.0038064339977193E-2</v>
+      </c>
+      <c r="O3">
+        <f>M2-M3</f>
+        <v>4931</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3154,6 +3206,21 @@
       <c r="G22">
         <v>154</v>
       </c>
+      <c r="J22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -3177,28 +3244,63 @@
       <c r="G23">
         <v>6</v>
       </c>
+      <c r="I23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <f>L2</f>
+        <v>143756</v>
+      </c>
+      <c r="K23">
+        <f>J6+J8</f>
+        <v>65059</v>
+      </c>
+      <c r="L23">
+        <f>J10+J12</f>
+        <v>20205</v>
+      </c>
+      <c r="M23">
+        <f>J14+J16</f>
+        <v>77155</v>
+      </c>
+      <c r="N23">
+        <f>J18+J20</f>
+        <v>8313</v>
+      </c>
+      <c r="O23">
+        <f>N23/J23</f>
+        <v>5.7827151562369568E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24">
-        <v>71</v>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="3">
+        <f>K3*100</f>
+        <v>0.28033612510086536</v>
+      </c>
+      <c r="K24" s="3">
+        <f>L7*100</f>
+        <v>0.38272952243348346</v>
+      </c>
+      <c r="L24" s="3">
+        <f>L11*100</f>
+        <v>0.46028210838901268</v>
+      </c>
+      <c r="M24" s="3">
+        <f>L15*100</f>
+        <v>0.31495042447022231</v>
+      </c>
+      <c r="N24" s="3">
+        <f>L19*100</f>
+        <v>0.6495849873691808</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -3218,33 +3320,79 @@
         <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>109</v>
+        <v>71</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="3">
+        <f>K2*100</f>
+        <v>5.8801023957260918</v>
+      </c>
+      <c r="K25" s="3">
+        <f>L6*100</f>
+        <v>8.1095620897954159</v>
+      </c>
+      <c r="L25" s="3">
+        <f>L10*100</f>
+        <v>9.200692897797575</v>
+      </c>
+      <c r="M25" s="3">
+        <f>L14*100</f>
+        <v>6.2134663988075953</v>
+      </c>
+      <c r="N25" s="3">
+        <f>L18*100</f>
+        <v>11.680500421027308</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G26">
-        <v>29883</v>
+        <v>109</v>
+      </c>
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="3">
+        <f>K4*100</f>
+        <v>94.119897604273902</v>
+      </c>
+      <c r="K26" s="3">
+        <f>L8*100</f>
+        <v>91.890437910204582</v>
+      </c>
+      <c r="L26" s="3">
+        <f>L12*100</f>
+        <v>90.79930710220242</v>
+      </c>
+      <c r="M26" s="3">
+        <f>L16*100</f>
+        <v>93.786533601192403</v>
+      </c>
+      <c r="N26" s="3">
+        <f>L20*100</f>
+        <v>88.319499578972696</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3264,10 +3412,10 @@
         <v>6</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G27">
-        <v>1931</v>
+        <v>29883</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -3284,13 +3432,28 @@
         <v>6</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G28">
-        <v>35680</v>
+        <v>1931</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3310,10 +3473,37 @@
         <v>7</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G29">
-        <v>8026</v>
+        <v>35680</v>
+      </c>
+      <c r="I29" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <f>O2</f>
+        <v>61638</v>
+      </c>
+      <c r="K29">
+        <f>M6+M8</f>
+        <v>26170</v>
+      </c>
+      <c r="L29">
+        <f>M10+M12</f>
+        <v>15404</v>
+      </c>
+      <c r="M29">
+        <f>M14+M16</f>
+        <v>25881</v>
+      </c>
+      <c r="N29">
+        <f>M18+M20</f>
+        <v>5517</v>
+      </c>
+      <c r="O29">
+        <f>N29/J29</f>
+        <v>8.950647327947045E-2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -3327,16 +3517,39 @@
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G30">
-        <v>30081</v>
+        <v>8026</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="3">
+        <f>N3*100</f>
+        <v>1.0038064339977193</v>
+      </c>
+      <c r="K30" s="3">
+        <f>O7*100</f>
+        <v>1.2991975544516623</v>
+      </c>
+      <c r="L30" s="3">
+        <f>L11*100</f>
+        <v>0.46028210838901268</v>
+      </c>
+      <c r="M30" s="3">
+        <f>O15*100</f>
+        <v>1.3252965495923652</v>
+      </c>
+      <c r="N30" s="3">
+        <f>O19*100</f>
+        <v>1.975711437375385</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -3356,10 +3569,33 @@
         <v>6</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G31">
-        <v>1047</v>
+        <v>30081</v>
+      </c>
+      <c r="I31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="3">
+        <f>N2*100</f>
+        <v>9.0139199844251916</v>
+      </c>
+      <c r="K31" s="3">
+        <f>O10*100</f>
+        <v>13.100493378343286</v>
+      </c>
+      <c r="L31" s="3">
+        <f>L10*100</f>
+        <v>9.200692897797575</v>
+      </c>
+      <c r="M31" s="3">
+        <f>O14*100</f>
+        <v>11.170356632278505</v>
+      </c>
+      <c r="N31" s="3">
+        <f>O18*100</f>
+        <v>15.515678810947978</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -3376,13 +3612,36 @@
         <v>7</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G32">
-        <v>21313</v>
+        <v>1047</v>
+      </c>
+      <c r="I32" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="3">
+        <f>N4*100</f>
+        <v>90.986080015574814</v>
+      </c>
+      <c r="K32" s="3">
+        <f>O8*100</f>
+        <v>88.696981276270535</v>
+      </c>
+      <c r="L32" s="3">
+        <f t="shared" ref="L31:L32" si="2">L12*100</f>
+        <v>90.79930710220242</v>
+      </c>
+      <c r="M32" s="3">
+        <f>O16*100</f>
+        <v>88.829643367721488</v>
+      </c>
+      <c r="N32" s="3">
+        <f>O20*100</f>
+        <v>84.484321189052025</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -3402,10 +3661,10 @@
         <v>7</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G33">
-        <v>7342</v>
+        <v>21313</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -3413,22 +3672,22 @@
         <v>7</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G34">
-        <v>1058</v>
+        <v>7342</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -3448,10 +3707,10 @@
         <v>6</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G35">
-        <v>167</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -3468,13 +3727,13 @@
         <v>6</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G36">
-        <v>1270</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -3494,10 +3753,10 @@
         <v>7</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G37">
-        <v>528</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -3511,16 +3770,16 @@
         <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G38">
-        <v>2120</v>
+        <v>528</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -3540,10 +3799,10 @@
         <v>6</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G39">
-        <v>154</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -3560,13 +3819,13 @@
         <v>7</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G40">
-        <v>1836</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -3586,10 +3845,10 @@
         <v>7</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G41">
-        <v>917</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -3600,19 +3859,19 @@
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G42">
-        <v>45</v>
+        <v>917</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -3632,10 +3891,10 @@
         <v>6</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G43">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -3652,13 +3911,13 @@
         <v>6</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G44">
-        <v>80</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -3678,10 +3937,10 @@
         <v>7</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G45">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -3695,16 +3954,16 @@
         <v>7</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G46">
-        <v>96</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -3724,10 +3983,10 @@
         <v>6</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G47">
-        <v>10</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -3744,13 +4003,13 @@
         <v>7</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G48">
-        <v>89</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -3770,9 +4029,32 @@
         <v>7</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G49">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50">
         <v>54</v>
       </c>
     </row>

</xml_diff>